<commit_message>
Add alteration functionality for almost same table and functionality to avoid data redundancy
</commit_message>
<xml_diff>
--- a/Backend/ExcelSql/Book.xlsx
+++ b/Backend/ExcelSql/Book.xlsx
@@ -5,72 +5,88 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\training\Excel-Sql\ExcelSql\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\training\excel_sql_git\Excel_SQL\Backend\ExcelSql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E9E120-02BA-41DC-9D0C-B26F2BAAF592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A048F57-A31B-4BEF-A075-74167FA9CA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-990" windowWidth="19440" windowHeight="10440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="510" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet Data" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
   <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
     <t>Age</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Mobile</t>
-  </si>
-  <si>
-    <t>Devesh</t>
-  </si>
-  <si>
-    <t>devesh@mail.com</t>
-  </si>
-  <si>
-    <t>Anjali</t>
-  </si>
-  <si>
-    <t>anjali@mail.com</t>
-  </si>
-  <si>
-    <t>Naina</t>
-  </si>
-  <si>
-    <t>naina@mail.com</t>
-  </si>
-  <si>
-    <t>Mudit</t>
-  </si>
-  <si>
-    <t>mudit@mail.com</t>
-  </si>
-  <si>
-    <t>Shreesh</t>
-  </si>
-  <si>
-    <t>nashe@mail.com</t>
-  </si>
-  <si>
-    <t>EmpID</t>
+    <t>Atul</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Ajay</t>
+  </si>
+  <si>
+    <t>ajay@mail.com</t>
+  </si>
+  <si>
+    <t>Mohit</t>
+  </si>
+  <si>
+    <t>mohit@mail.com</t>
+  </si>
+  <si>
+    <t>Saif</t>
+  </si>
+  <si>
+    <t>said@mail.com</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>Riya</t>
+  </si>
+  <si>
+    <t>riya@mail.com</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -398,162 +414,138 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F78ED1B2-E011-4E4B-B79B-3C2281E84064}">
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>34264325</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
-        <v>69</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>6969696969</v>
+      <c r="B3">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>354856</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>9238953</v>
+      </c>
+      <c r="E4" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
-        <v>96</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3">
-        <v>9696969696</v>
-      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4">
-        <v>150</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4">
-        <v>8989729384</v>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>27</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>895238752</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>20</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5">
-        <v>7588485938</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B6">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D6">
-        <v>9845857848</v>
+        <v>8732957</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6">
+        <v>20000</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{E12BC887-CC2A-4115-8D28-237BE0DEBC23}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{A0F8B7C3-F271-418C-94C2-933496D2197C}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{CAEE04A2-A465-485C-988D-8AE82331C46B}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{CFEFCC91-8F0E-4178-ABF2-63662C5D5C46}"/>
-    <hyperlink ref="C6" r:id="rId5" xr:uid="{D7DC96BA-AD1C-42CD-9866-AD6A6AC34432}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{6FB316A0-6318-4A61-921E-BBF1E59C4DCB}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{063CF342-B83E-4E6F-9DAB-9153676882B7}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{FFE6F810-F2F9-46A7-BD36-C1258DA0E05E}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{E2F8E050-A694-45E3-A27C-13D1E7E8ADAD}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{A5616025-4D41-4881-978D-4D3DD562D643}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE75E063-4AD5-4A4E-BD65-1C2000A446B1}">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>910</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>8985849</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>906</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3">
-        <v>759834895</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add data duplicity validation on backend
</commit_message>
<xml_diff>
--- a/Backend/ExcelSql/Book.xlsx
+++ b/Backend/ExcelSql/Book.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\training\excel_sql_git\Excel_SQL\Backend\ExcelSql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A048F57-A31B-4BEF-A075-74167FA9CA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD4EA0E-1396-40D3-A3FF-D0A85B89559C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="510" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24435" yWindow="1635" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet Data" sheetId="3" r:id="rId1"/>
+    <sheet name="ABC" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -87,6 +88,18 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Rohit</t>
+  </si>
+  <si>
+    <t>rohit@mail</t>
+  </si>
+  <si>
+    <t>Noida</t>
   </si>
 </sst>
 </file>
@@ -417,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F78ED1B2-E011-4E4B-B79B-3C2281E84064}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,4 +561,68 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B4264C8-A42E-4FC2-A784-0F8006783A50}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>26</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2">
+        <v>398539</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <v>3000</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{C7CCF92D-4E68-45E4-AE7C-3B6F6131AD03}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>